<commit_message>
fix: - material shoe up linen edit
</commit_message>
<xml_diff>
--- a/app/download_dir/system_files/обувь_по каждому размеру.xlsx
+++ b/app/download_dir/system_files/обувь_по каждому размеру.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1595" uniqueCount="854">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1591" uniqueCount="852">
   <si>
     <t xml:space="preserve">Код ТНВЭД</t>
   </si>
@@ -1362,9 +1362,6 @@
     <t xml:space="preserve">Парусина</t>
   </si>
   <si>
-    <t xml:space="preserve">Джинс</t>
-  </si>
-  <si>
     <t xml:space="preserve">Войлок</t>
   </si>
   <si>
@@ -1381,9 +1378,6 @@
   </si>
   <si>
     <t xml:space="preserve">Хлопок</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Сетчатое полотно</t>
   </si>
   <si>
     <t xml:space="preserve">Искусственная замша</t>
@@ -3819,10 +3813,10 @@
   <dimension ref="A1:AC1035"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
+      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.1015625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.12109375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="44.04"/>
@@ -3838,7 +3832,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="17.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="11.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="11.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="7.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="7.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="3" width="11.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="8.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="7.39"/>
@@ -4285,7 +4279,7 @@
       <c r="A9" s="30"/>
       <c r="B9" s="31" t="str">
         <f aca="false">CONCATENATE(F9, " ", C9, " арт. ", E9, " цвет. ", G9, " р.", H9)</f>
-        <v>  арт.  цвет.  р.</v>
+        <v>арт.  цвет.  р.</v>
       </c>
       <c r="C9" s="32"/>
       <c r="D9" s="33" t="s">
@@ -4310,7 +4304,7 @@
       <c r="A10" s="30"/>
       <c r="B10" s="31" t="str">
         <f aca="false">CONCATENATE(F10, " ", C10, " арт. ", E10, " цвет. ", G10, " р.", H10)</f>
-        <v>  арт.  цвет.  р.</v>
+        <v>арт.  цвет.  р.</v>
       </c>
       <c r="C10" s="32"/>
       <c r="D10" s="33" t="s">
@@ -4335,7 +4329,7 @@
       <c r="A11" s="30"/>
       <c r="B11" s="31" t="str">
         <f aca="false">CONCATENATE(F11, " ", C11, " арт. ", E11, " цвет. ", G11, " р.", H11)</f>
-        <v>  арт.  цвет.  р.</v>
+        <v>арт.  цвет.  р.</v>
       </c>
       <c r="C11" s="32"/>
       <c r="D11" s="33" t="s">
@@ -4360,7 +4354,7 @@
       <c r="A12" s="30"/>
       <c r="B12" s="31" t="str">
         <f aca="false">CONCATENATE(F12, " ", C12, " арт. ", E12, " цвет. ", G12, " р.", H12)</f>
-        <v>  арт.  цвет.  р.</v>
+        <v>арт.  цвет.  р.</v>
       </c>
       <c r="C12" s="32"/>
       <c r="D12" s="33" t="s">
@@ -4385,7 +4379,7 @@
       <c r="A13" s="30"/>
       <c r="B13" s="31" t="str">
         <f aca="false">CONCATENATE(F13, " ", C13, " арт. ", E13, " цвет. ", G13, " р.", H13)</f>
-        <v>  арт.  цвет.  р.</v>
+        <v>арт.  цвет.  р.</v>
       </c>
       <c r="C13" s="32"/>
       <c r="D13" s="33" t="s">
@@ -4410,7 +4404,7 @@
       <c r="A14" s="30"/>
       <c r="B14" s="31" t="str">
         <f aca="false">CONCATENATE(F14, " ", C14, " арт. ", E14, " цвет. ", G14, " р.", H14)</f>
-        <v>  арт.  цвет.  р.</v>
+        <v>арт.  цвет.  р.</v>
       </c>
       <c r="C14" s="32"/>
       <c r="D14" s="33" t="s">
@@ -4435,7 +4429,7 @@
       <c r="A15" s="30"/>
       <c r="B15" s="31" t="str">
         <f aca="false">CONCATENATE(F15, " ", C15, " арт. ", E15, " цвет. ", G15, " р.", H15)</f>
-        <v>  арт.  цвет.  р.</v>
+        <v>арт.  цвет.  р.</v>
       </c>
       <c r="C15" s="32"/>
       <c r="D15" s="33" t="s">
@@ -4460,7 +4454,7 @@
       <c r="A16" s="30"/>
       <c r="B16" s="31" t="str">
         <f aca="false">CONCATENATE(F16, " ", C16, " арт. ", E16, " цвет. ", G16, " р.", H16)</f>
-        <v>  арт.  цвет.  р.</v>
+        <v>арт.  цвет.  р.</v>
       </c>
       <c r="C16" s="32"/>
       <c r="D16" s="33" t="s">
@@ -4485,7 +4479,7 @@
       <c r="A17" s="30"/>
       <c r="B17" s="31" t="str">
         <f aca="false">CONCATENATE(F17, " ", C17, " арт. ", E17, " цвет. ", G17, " р.", H17)</f>
-        <v>  арт.  цвет.  р.</v>
+        <v>арт.  цвет.  р.</v>
       </c>
       <c r="C17" s="32"/>
       <c r="D17" s="33" t="s">
@@ -4510,7 +4504,7 @@
       <c r="A18" s="30"/>
       <c r="B18" s="31" t="str">
         <f aca="false">CONCATENATE(F18, " ", C18, " арт. ", E18, " цвет. ", G18, " р.", H18)</f>
-        <v>  арт.  цвет.  р.</v>
+        <v>арт.  цвет.  р.</v>
       </c>
       <c r="C18" s="32"/>
       <c r="D18" s="33" t="s">
@@ -4535,7 +4529,7 @@
       <c r="A19" s="30"/>
       <c r="B19" s="31" t="str">
         <f aca="false">CONCATENATE(F19, " ", C19, " арт. ", E19, " цвет. ", G19, " р.", H19)</f>
-        <v>  арт.  цвет.  р.</v>
+        <v>арт.  цвет.  р.</v>
       </c>
       <c r="C19" s="32"/>
       <c r="D19" s="33" t="s">
@@ -4560,7 +4554,7 @@
       <c r="A20" s="30"/>
       <c r="B20" s="31" t="str">
         <f aca="false">CONCATENATE(F20, " ", C20, " арт. ", E20, " цвет. ", G20, " р.", H20)</f>
-        <v>  арт.  цвет.  р.</v>
+        <v>арт.  цвет.  р.</v>
       </c>
       <c r="C20" s="32"/>
       <c r="D20" s="33" t="s">
@@ -4585,7 +4579,7 @@
       <c r="A21" s="30"/>
       <c r="B21" s="31" t="str">
         <f aca="false">CONCATENATE(F21, " ", C21, " арт. ", E21, " цвет. ", G21, " р.", H21)</f>
-        <v>  арт.  цвет.  р.</v>
+        <v>арт.  цвет.  р.</v>
       </c>
       <c r="C21" s="32"/>
       <c r="D21" s="33" t="s">
@@ -4610,7 +4604,7 @@
       <c r="A22" s="30"/>
       <c r="B22" s="31" t="str">
         <f aca="false">CONCATENATE(F22, " ", C22, " арт. ", E22, " цвет. ", G22, " р.", H22)</f>
-        <v>  арт.  цвет.  р.</v>
+        <v>арт.  цвет.  р.</v>
       </c>
       <c r="C22" s="32"/>
       <c r="D22" s="33" t="s">
@@ -4635,7 +4629,7 @@
       <c r="A23" s="30"/>
       <c r="B23" s="31" t="str">
         <f aca="false">CONCATENATE(F23, " ", C23, " арт. ", E23, " цвет. ", G23, " р.", H23)</f>
-        <v>  арт.  цвет.  р.</v>
+        <v>арт.  цвет.  р.</v>
       </c>
       <c r="C23" s="32"/>
       <c r="D23" s="33" t="s">
@@ -4660,7 +4654,7 @@
       <c r="A24" s="30"/>
       <c r="B24" s="31" t="str">
         <f aca="false">CONCATENATE(F24, " ", C24, " арт. ", E24, " цвет. ", G24, " р.", H24)</f>
-        <v>  арт.  цвет.  р.</v>
+        <v>арт.  цвет.  р.</v>
       </c>
       <c r="C24" s="32"/>
       <c r="D24" s="33" t="s">
@@ -4685,7 +4679,7 @@
       <c r="A25" s="30"/>
       <c r="B25" s="31" t="str">
         <f aca="false">CONCATENATE(F25, " ", C25, " арт. ", E25, " цвет. ", G25, " р.", H25)</f>
-        <v>  арт.  цвет.  р.</v>
+        <v>арт.  цвет.  р.</v>
       </c>
       <c r="C25" s="32"/>
       <c r="D25" s="33" t="s">
@@ -4710,7 +4704,7 @@
       <c r="A26" s="30"/>
       <c r="B26" s="31" t="str">
         <f aca="false">CONCATENATE(F26, " ", C26, " арт. ", E26, " цвет. ", G26, " р.", H26)</f>
-        <v>  арт.  цвет.  р.</v>
+        <v>арт.  цвет.  р.</v>
       </c>
       <c r="C26" s="32"/>
       <c r="D26" s="33" t="s">
@@ -4735,7 +4729,7 @@
       <c r="A27" s="30"/>
       <c r="B27" s="31" t="str">
         <f aca="false">CONCATENATE(F27, " ", C27, " арт. ", E27, " цвет. ", G27, " р.", H27)</f>
-        <v>  арт.  цвет.  р.</v>
+        <v>арт.  цвет.  р.</v>
       </c>
       <c r="C27" s="32"/>
       <c r="D27" s="33" t="s">
@@ -4760,7 +4754,7 @@
       <c r="A28" s="30"/>
       <c r="B28" s="31" t="str">
         <f aca="false">CONCATENATE(F28, " ", C28, " арт. ", E28, " цвет. ", G28, " р.", H28)</f>
-        <v>  арт.  цвет.  р.</v>
+        <v>арт.  цвет.  р.</v>
       </c>
       <c r="C28" s="32"/>
       <c r="D28" s="33" t="s">
@@ -4785,7 +4779,7 @@
       <c r="A29" s="30"/>
       <c r="B29" s="31" t="str">
         <f aca="false">CONCATENATE(F29, " ", C29, " арт. ", E29, " цвет. ", G29, " р.", H29)</f>
-        <v>  арт.  цвет.  р.</v>
+        <v>арт.  цвет.  р.</v>
       </c>
       <c r="C29" s="32"/>
       <c r="D29" s="33" t="s">
@@ -4810,7 +4804,7 @@
       <c r="A30" s="30"/>
       <c r="B30" s="31" t="str">
         <f aca="false">CONCATENATE(F30, " ", C30, " арт. ", E30, " цвет. ", G30, " р.", H30)</f>
-        <v>  арт.  цвет.  р.</v>
+        <v>арт.  цвет.  р.</v>
       </c>
       <c r="C30" s="32"/>
       <c r="D30" s="33" t="s">
@@ -4835,7 +4829,7 @@
       <c r="A31" s="30"/>
       <c r="B31" s="31" t="str">
         <f aca="false">CONCATENATE(F31, " ", C31, " арт. ", E31, " цвет. ", G31, " р.", H31)</f>
-        <v>  арт.  цвет.  р.</v>
+        <v>арт.  цвет.  р.</v>
       </c>
       <c r="C31" s="32"/>
       <c r="D31" s="33" t="s">
@@ -4860,7 +4854,7 @@
       <c r="A32" s="30"/>
       <c r="B32" s="31" t="str">
         <f aca="false">CONCATENATE(F32, " ", C32, " арт. ", E32, " цвет. ", G32, " р.", H32)</f>
-        <v>  арт.  цвет.  р.</v>
+        <v>арт.  цвет.  р.</v>
       </c>
       <c r="C32" s="32"/>
       <c r="D32" s="33" t="s">
@@ -4885,7 +4879,7 @@
       <c r="A33" s="30"/>
       <c r="B33" s="24" t="str">
         <f aca="false">CONCATENATE(F33, " ", C33, " арт. ", E33, " цвет. ", G33, " р.", H33)</f>
-        <v>  арт.  цвет.  р.</v>
+        <v>арт.  цвет.  р.</v>
       </c>
       <c r="C33" s="32"/>
       <c r="D33" s="33" t="s">
@@ -18673,19 +18667,19 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="T7" type="list">
-      <formula1>Справочники!$B$435:$B$675</formula1>
+      <formula1>Справочники!$B$433:$B$673</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="I7:J1034" type="list">
-      <formula1>Справочники!$B$366:$B$406</formula1>
+      <formula1>Справочники!$B$366:$B$404</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="U7:U1034" type="list">
-      <formula1>Справочники!$B$678:$B$680</formula1>
+      <formula1>Справочники!$B$676:$B$678</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="T9:T1034" type="list">
-      <formula1>Справочники!$B$435:$B$675</formula1>
+      <formula1>Справочники!$B$433:$B$673</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F7:F8" type="list">
@@ -18709,7 +18703,7 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="T8" type="list">
-      <formula1>Справочники!$B$435:$B$675</formula1>
+      <formula1>Справочники!$B$433:$B$673</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="lessThan" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B6" type="textLength">
@@ -18717,11 +18711,11 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="K7:K1034" type="list">
-      <formula1>Справочники!$B$410:$B$424</formula1>
+      <formula1>Справочники!$B$408:$B$422</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O7:O1034" type="list">
-      <formula1>Справочники!$B$427:$B$432</formula1>
+      <formula1>Справочники!$B$425:$B$430</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="lessThan" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C5 B34" type="textLength">
@@ -18744,13 +18738,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B680"/>
+  <dimension ref="A1:B678"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A349" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B364" activeCellId="0" sqref="B364"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A382" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B402" activeCellId="0" sqref="B402"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.1015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.12109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="63.59"/>
@@ -21827,7 +21821,7 @@
       <c r="A394" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="B394" s="1" t="s">
+      <c r="B394" s="49" t="s">
         <v>451</v>
       </c>
     </row>
@@ -21843,7 +21837,7 @@
       <c r="A396" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="B396" s="49" t="s">
+      <c r="B396" s="1" t="s">
         <v>453</v>
       </c>
     </row>
@@ -21851,17 +21845,11 @@
       <c r="A397" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="B397" s="1" t="s">
-        <v>454</v>
-      </c>
     </row>
     <row r="398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="B398" s="1" t="s">
-        <v>455</v>
-      </c>
     </row>
     <row r="399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="1" t="s">
@@ -21893,187 +21881,193 @@
         <v>425</v>
       </c>
     </row>
-    <row r="405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A405" s="1" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A406" s="1" t="s">
-        <v>425</v>
+    <row r="408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A408" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="B408" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A409" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="B409" s="1" t="s">
+        <v>455</v>
       </c>
     </row>
     <row r="410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B410" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
     </row>
     <row r="411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A411" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="B411" s="1" t="s">
         <v>456</v>
-      </c>
-      <c r="B411" s="1" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B412" s="1" t="s">
-        <v>73</v>
+        <v>432</v>
       </c>
     </row>
     <row r="413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B413" s="1" t="s">
-        <v>458</v>
+        <v>429</v>
       </c>
     </row>
     <row r="414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B414" s="1" t="s">
-        <v>432</v>
+        <v>457</v>
       </c>
     </row>
     <row r="415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A415" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B415" s="1" t="s">
-        <v>429</v>
+        <v>63</v>
       </c>
     </row>
     <row r="416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B416" s="1" t="s">
-        <v>459</v>
+        <v>430</v>
       </c>
     </row>
     <row r="417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B417" s="1" t="s">
-        <v>63</v>
+        <v>433</v>
       </c>
     </row>
     <row r="418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B418" s="1" t="s">
-        <v>430</v>
+        <v>450</v>
       </c>
     </row>
     <row r="419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A419" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B419" s="1" t="s">
-        <v>433</v>
+        <v>451</v>
       </c>
     </row>
     <row r="420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B420" s="1" t="s">
-        <v>452</v>
+        <v>458</v>
       </c>
     </row>
     <row r="421" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B421" s="1" t="s">
-        <v>453</v>
+        <v>444</v>
       </c>
     </row>
     <row r="422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B422" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="425" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A425" s="1" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="423" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A423" s="1" t="s">
-        <v>456</v>
-      </c>
-      <c r="B423" s="1" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="424" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A424" s="1" t="s">
-        <v>456</v>
-      </c>
-      <c r="B424" s="1" t="s">
+      <c r="B425" s="1" t="s">
         <v>461</v>
+      </c>
+    </row>
+    <row r="426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A426" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="B426" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B427" s="1" t="s">
-        <v>463</v>
+        <v>74</v>
       </c>
     </row>
     <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="B428" s="1" t="s">
         <v>462</v>
-      </c>
-      <c r="B428" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B429" s="1" t="s">
-        <v>74</v>
+        <v>463</v>
       </c>
     </row>
     <row r="430" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B430" s="1" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A431" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="B431" s="1" t="s">
+    <row r="433" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A433" s="1" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="432" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A432" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="B432" s="1" t="s">
+      <c r="B433" s="50" t="s">
         <v>466</v>
+      </c>
+    </row>
+    <row r="434" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A434" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="B434" s="50" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="435" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A435" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B435" s="50" t="s">
         <v>468</v>
@@ -22081,7 +22075,7 @@
     </row>
     <row r="436" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A436" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B436" s="50" t="s">
         <v>469</v>
@@ -22089,7 +22083,7 @@
     </row>
     <row r="437" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A437" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B437" s="50" t="s">
         <v>470</v>
@@ -22097,7 +22091,7 @@
     </row>
     <row r="438" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B438" s="50" t="s">
         <v>471</v>
@@ -22105,7 +22099,7 @@
     </row>
     <row r="439" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B439" s="50" t="s">
         <v>472</v>
@@ -22113,7 +22107,7 @@
     </row>
     <row r="440" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B440" s="50" t="s">
         <v>473</v>
@@ -22121,7 +22115,7 @@
     </row>
     <row r="441" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B441" s="50" t="s">
         <v>474</v>
@@ -22129,7 +22123,7 @@
     </row>
     <row r="442" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B442" s="50" t="s">
         <v>475</v>
@@ -22137,7 +22131,7 @@
     </row>
     <row r="443" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A443" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B443" s="50" t="s">
         <v>476</v>
@@ -22145,7 +22139,7 @@
     </row>
     <row r="444" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A444" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B444" s="50" t="s">
         <v>477</v>
@@ -22153,7 +22147,7 @@
     </row>
     <row r="445" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A445" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B445" s="50" t="s">
         <v>478</v>
@@ -22161,7 +22155,7 @@
     </row>
     <row r="446" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A446" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B446" s="50" t="s">
         <v>479</v>
@@ -22169,7 +22163,7 @@
     </row>
     <row r="447" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A447" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B447" s="50" t="s">
         <v>480</v>
@@ -22177,7 +22171,7 @@
     </row>
     <row r="448" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A448" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B448" s="50" t="s">
         <v>481</v>
@@ -22185,7 +22179,7 @@
     </row>
     <row r="449" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A449" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B449" s="50" t="s">
         <v>482</v>
@@ -22193,7 +22187,7 @@
     </row>
     <row r="450" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A450" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B450" s="50" t="s">
         <v>483</v>
@@ -22201,7 +22195,7 @@
     </row>
     <row r="451" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A451" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B451" s="50" t="s">
         <v>484</v>
@@ -22209,7 +22203,7 @@
     </row>
     <row r="452" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A452" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B452" s="50" t="s">
         <v>485</v>
@@ -22217,7 +22211,7 @@
     </row>
     <row r="453" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A453" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B453" s="50" t="s">
         <v>486</v>
@@ -22225,7 +22219,7 @@
     </row>
     <row r="454" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A454" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B454" s="50" t="s">
         <v>487</v>
@@ -22233,7 +22227,7 @@
     </row>
     <row r="455" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A455" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B455" s="50" t="s">
         <v>488</v>
@@ -22241,7 +22235,7 @@
     </row>
     <row r="456" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A456" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B456" s="50" t="s">
         <v>489</v>
@@ -22249,7 +22243,7 @@
     </row>
     <row r="457" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A457" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B457" s="50" t="s">
         <v>490</v>
@@ -22257,7 +22251,7 @@
     </row>
     <row r="458" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A458" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B458" s="50" t="s">
         <v>491</v>
@@ -22265,7 +22259,7 @@
     </row>
     <row r="459" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A459" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B459" s="50" t="s">
         <v>492</v>
@@ -22273,7 +22267,7 @@
     </row>
     <row r="460" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A460" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B460" s="50" t="s">
         <v>493</v>
@@ -22281,7 +22275,7 @@
     </row>
     <row r="461" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A461" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B461" s="50" t="s">
         <v>494</v>
@@ -22289,7 +22283,7 @@
     </row>
     <row r="462" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A462" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B462" s="50" t="s">
         <v>495</v>
@@ -22297,7 +22291,7 @@
     </row>
     <row r="463" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A463" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B463" s="50" t="s">
         <v>496</v>
@@ -22305,7 +22299,7 @@
     </row>
     <row r="464" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A464" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B464" s="50" t="s">
         <v>497</v>
@@ -22313,7 +22307,7 @@
     </row>
     <row r="465" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A465" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B465" s="50" t="s">
         <v>498</v>
@@ -22321,7 +22315,7 @@
     </row>
     <row r="466" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A466" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B466" s="50" t="s">
         <v>499</v>
@@ -22329,7 +22323,7 @@
     </row>
     <row r="467" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A467" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B467" s="50" t="s">
         <v>500</v>
@@ -22337,7 +22331,7 @@
     </row>
     <row r="468" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A468" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B468" s="50" t="s">
         <v>501</v>
@@ -22345,7 +22339,7 @@
     </row>
     <row r="469" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A469" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B469" s="50" t="s">
         <v>502</v>
@@ -22353,7 +22347,7 @@
     </row>
     <row r="470" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A470" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B470" s="50" t="s">
         <v>503</v>
@@ -22361,7 +22355,7 @@
     </row>
     <row r="471" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A471" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B471" s="50" t="s">
         <v>504</v>
@@ -22369,7 +22363,7 @@
     </row>
     <row r="472" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A472" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B472" s="50" t="s">
         <v>505</v>
@@ -22377,7 +22371,7 @@
     </row>
     <row r="473" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A473" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B473" s="50" t="s">
         <v>506</v>
@@ -22385,7 +22379,7 @@
     </row>
     <row r="474" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A474" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B474" s="50" t="s">
         <v>507</v>
@@ -22393,7 +22387,7 @@
     </row>
     <row r="475" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A475" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B475" s="50" t="s">
         <v>508</v>
@@ -22401,7 +22395,7 @@
     </row>
     <row r="476" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A476" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B476" s="50" t="s">
         <v>509</v>
@@ -22409,7 +22403,7 @@
     </row>
     <row r="477" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A477" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B477" s="50" t="s">
         <v>510</v>
@@ -22417,31 +22411,31 @@
     </row>
     <row r="478" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A478" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B478" s="50" t="s">
-        <v>511</v>
+        <v>75</v>
       </c>
     </row>
     <row r="479" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A479" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B479" s="50" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="480" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A480" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B480" s="50" t="s">
-        <v>75</v>
+        <v>512</v>
       </c>
     </row>
     <row r="481" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A481" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B481" s="50" t="s">
         <v>513</v>
@@ -22449,7 +22443,7 @@
     </row>
     <row r="482" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A482" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B482" s="50" t="s">
         <v>514</v>
@@ -22457,7 +22451,7 @@
     </row>
     <row r="483" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A483" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B483" s="50" t="s">
         <v>515</v>
@@ -22465,7 +22459,7 @@
     </row>
     <row r="484" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A484" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B484" s="50" t="s">
         <v>516</v>
@@ -22473,7 +22467,7 @@
     </row>
     <row r="485" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A485" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B485" s="50" t="s">
         <v>517</v>
@@ -22481,7 +22475,7 @@
     </row>
     <row r="486" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A486" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B486" s="50" t="s">
         <v>518</v>
@@ -22489,7 +22483,7 @@
     </row>
     <row r="487" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A487" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B487" s="50" t="s">
         <v>519</v>
@@ -22497,7 +22491,7 @@
     </row>
     <row r="488" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A488" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B488" s="50" t="s">
         <v>520</v>
@@ -22505,7 +22499,7 @@
     </row>
     <row r="489" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A489" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B489" s="50" t="s">
         <v>521</v>
@@ -22513,7 +22507,7 @@
     </row>
     <row r="490" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A490" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B490" s="50" t="s">
         <v>522</v>
@@ -22521,7 +22515,7 @@
     </row>
     <row r="491" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A491" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B491" s="50" t="s">
         <v>523</v>
@@ -22529,7 +22523,7 @@
     </row>
     <row r="492" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A492" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B492" s="50" t="s">
         <v>524</v>
@@ -22537,7 +22531,7 @@
     </row>
     <row r="493" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A493" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B493" s="50" t="s">
         <v>525</v>
@@ -22545,7 +22539,7 @@
     </row>
     <row r="494" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A494" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B494" s="50" t="s">
         <v>526</v>
@@ -22553,7 +22547,7 @@
     </row>
     <row r="495" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A495" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B495" s="50" t="s">
         <v>527</v>
@@ -22561,7 +22555,7 @@
     </row>
     <row r="496" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A496" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B496" s="50" t="s">
         <v>528</v>
@@ -22569,7 +22563,7 @@
     </row>
     <row r="497" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A497" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B497" s="50" t="s">
         <v>529</v>
@@ -22577,7 +22571,7 @@
     </row>
     <row r="498" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A498" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B498" s="50" t="s">
         <v>530</v>
@@ -22585,7 +22579,7 @@
     </row>
     <row r="499" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A499" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B499" s="50" t="s">
         <v>531</v>
@@ -22593,7 +22587,7 @@
     </row>
     <row r="500" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A500" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B500" s="50" t="s">
         <v>532</v>
@@ -22601,7 +22595,7 @@
     </row>
     <row r="501" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A501" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B501" s="50" t="s">
         <v>533</v>
@@ -22609,7 +22603,7 @@
     </row>
     <row r="502" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A502" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B502" s="50" t="s">
         <v>534</v>
@@ -22617,7 +22611,7 @@
     </row>
     <row r="503" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A503" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B503" s="50" t="s">
         <v>535</v>
@@ -22625,7 +22619,7 @@
     </row>
     <row r="504" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A504" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B504" s="50" t="s">
         <v>536</v>
@@ -22633,7 +22627,7 @@
     </row>
     <row r="505" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A505" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B505" s="50" t="s">
         <v>537</v>
@@ -22641,7 +22635,7 @@
     </row>
     <row r="506" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A506" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B506" s="50" t="s">
         <v>538</v>
@@ -22649,7 +22643,7 @@
     </row>
     <row r="507" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A507" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B507" s="50" t="s">
         <v>539</v>
@@ -22657,7 +22651,7 @@
     </row>
     <row r="508" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A508" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B508" s="50" t="s">
         <v>540</v>
@@ -22665,7 +22659,7 @@
     </row>
     <row r="509" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A509" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B509" s="50" t="s">
         <v>541</v>
@@ -22673,7 +22667,7 @@
     </row>
     <row r="510" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A510" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B510" s="50" t="s">
         <v>542</v>
@@ -22681,7 +22675,7 @@
     </row>
     <row r="511" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A511" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B511" s="50" t="s">
         <v>543</v>
@@ -22689,7 +22683,7 @@
     </row>
     <row r="512" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A512" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B512" s="50" t="s">
         <v>544</v>
@@ -22697,7 +22691,7 @@
     </row>
     <row r="513" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A513" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B513" s="50" t="s">
         <v>545</v>
@@ -22705,7 +22699,7 @@
     </row>
     <row r="514" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A514" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B514" s="50" t="s">
         <v>546</v>
@@ -22713,7 +22707,7 @@
     </row>
     <row r="515" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A515" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B515" s="50" t="s">
         <v>547</v>
@@ -22721,7 +22715,7 @@
     </row>
     <row r="516" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A516" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B516" s="50" t="s">
         <v>548</v>
@@ -22729,7 +22723,7 @@
     </row>
     <row r="517" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A517" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B517" s="50" t="s">
         <v>549</v>
@@ -22737,7 +22731,7 @@
     </row>
     <row r="518" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A518" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B518" s="50" t="s">
         <v>550</v>
@@ -22745,7 +22739,7 @@
     </row>
     <row r="519" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A519" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B519" s="50" t="s">
         <v>551</v>
@@ -22753,7 +22747,7 @@
     </row>
     <row r="520" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A520" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B520" s="50" t="s">
         <v>552</v>
@@ -22761,7 +22755,7 @@
     </row>
     <row r="521" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A521" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B521" s="50" t="s">
         <v>553</v>
@@ -22769,7 +22763,7 @@
     </row>
     <row r="522" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A522" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B522" s="50" t="s">
         <v>554</v>
@@ -22777,7 +22771,7 @@
     </row>
     <row r="523" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A523" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B523" s="50" t="s">
         <v>555</v>
@@ -22785,7 +22779,7 @@
     </row>
     <row r="524" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A524" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B524" s="50" t="s">
         <v>556</v>
@@ -22793,7 +22787,7 @@
     </row>
     <row r="525" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A525" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B525" s="50" t="s">
         <v>557</v>
@@ -22801,7 +22795,7 @@
     </row>
     <row r="526" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A526" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B526" s="50" t="s">
         <v>558</v>
@@ -22809,7 +22803,7 @@
     </row>
     <row r="527" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A527" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B527" s="50" t="s">
         <v>559</v>
@@ -22817,7 +22811,7 @@
     </row>
     <row r="528" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A528" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B528" s="50" t="s">
         <v>560</v>
@@ -22825,7 +22819,7 @@
     </row>
     <row r="529" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A529" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B529" s="50" t="s">
         <v>561</v>
@@ -22833,7 +22827,7 @@
     </row>
     <row r="530" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A530" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B530" s="50" t="s">
         <v>562</v>
@@ -22841,7 +22835,7 @@
     </row>
     <row r="531" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A531" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B531" s="50" t="s">
         <v>563</v>
@@ -22849,7 +22843,7 @@
     </row>
     <row r="532" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A532" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B532" s="50" t="s">
         <v>564</v>
@@ -22857,7 +22851,7 @@
     </row>
     <row r="533" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A533" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B533" s="50" t="s">
         <v>565</v>
@@ -22865,7 +22859,7 @@
     </row>
     <row r="534" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A534" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B534" s="50" t="s">
         <v>566</v>
@@ -22873,7 +22867,7 @@
     </row>
     <row r="535" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A535" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B535" s="50" t="s">
         <v>567</v>
@@ -22881,7 +22875,7 @@
     </row>
     <row r="536" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A536" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B536" s="50" t="s">
         <v>568</v>
@@ -22889,7 +22883,7 @@
     </row>
     <row r="537" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A537" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B537" s="50" t="s">
         <v>569</v>
@@ -22897,7 +22891,7 @@
     </row>
     <row r="538" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A538" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B538" s="50" t="s">
         <v>570</v>
@@ -22905,7 +22899,7 @@
     </row>
     <row r="539" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A539" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B539" s="50" t="s">
         <v>571</v>
@@ -22913,7 +22907,7 @@
     </row>
     <row r="540" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A540" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B540" s="50" t="s">
         <v>572</v>
@@ -22921,7 +22915,7 @@
     </row>
     <row r="541" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A541" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B541" s="50" t="s">
         <v>573</v>
@@ -22929,7 +22923,7 @@
     </row>
     <row r="542" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A542" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B542" s="50" t="s">
         <v>574</v>
@@ -22937,7 +22931,7 @@
     </row>
     <row r="543" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A543" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B543" s="50" t="s">
         <v>575</v>
@@ -22945,7 +22939,7 @@
     </row>
     <row r="544" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A544" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B544" s="50" t="s">
         <v>576</v>
@@ -22953,7 +22947,7 @@
     </row>
     <row r="545" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A545" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B545" s="50" t="s">
         <v>577</v>
@@ -22961,7 +22955,7 @@
     </row>
     <row r="546" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A546" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B546" s="50" t="s">
         <v>578</v>
@@ -22969,7 +22963,7 @@
     </row>
     <row r="547" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A547" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B547" s="50" t="s">
         <v>579</v>
@@ -22977,7 +22971,7 @@
     </row>
     <row r="548" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A548" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B548" s="50" t="s">
         <v>580</v>
@@ -22985,7 +22979,7 @@
     </row>
     <row r="549" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A549" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B549" s="50" t="s">
         <v>581</v>
@@ -22993,7 +22987,7 @@
     </row>
     <row r="550" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A550" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B550" s="50" t="s">
         <v>582</v>
@@ -23001,7 +22995,7 @@
     </row>
     <row r="551" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A551" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B551" s="50" t="s">
         <v>583</v>
@@ -23009,7 +23003,7 @@
     </row>
     <row r="552" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A552" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B552" s="50" t="s">
         <v>584</v>
@@ -23017,7 +23011,7 @@
     </row>
     <row r="553" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A553" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B553" s="50" t="s">
         <v>585</v>
@@ -23025,7 +23019,7 @@
     </row>
     <row r="554" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A554" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B554" s="50" t="s">
         <v>586</v>
@@ -23033,7 +23027,7 @@
     </row>
     <row r="555" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A555" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B555" s="50" t="s">
         <v>587</v>
@@ -23041,7 +23035,7 @@
     </row>
     <row r="556" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A556" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B556" s="50" t="s">
         <v>588</v>
@@ -23049,7 +23043,7 @@
     </row>
     <row r="557" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A557" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B557" s="50" t="s">
         <v>589</v>
@@ -23057,7 +23051,7 @@
     </row>
     <row r="558" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A558" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B558" s="50" t="s">
         <v>590</v>
@@ -23065,7 +23059,7 @@
     </row>
     <row r="559" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A559" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B559" s="50" t="s">
         <v>591</v>
@@ -23073,7 +23067,7 @@
     </row>
     <row r="560" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A560" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B560" s="50" t="s">
         <v>592</v>
@@ -23081,7 +23075,7 @@
     </row>
     <row r="561" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A561" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B561" s="50" t="s">
         <v>593</v>
@@ -23089,7 +23083,7 @@
     </row>
     <row r="562" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A562" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B562" s="50" t="s">
         <v>594</v>
@@ -23097,7 +23091,7 @@
     </row>
     <row r="563" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A563" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B563" s="50" t="s">
         <v>595</v>
@@ -23105,7 +23099,7 @@
     </row>
     <row r="564" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A564" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B564" s="50" t="s">
         <v>596</v>
@@ -23113,7 +23107,7 @@
     </row>
     <row r="565" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A565" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B565" s="50" t="s">
         <v>597</v>
@@ -23121,7 +23115,7 @@
     </row>
     <row r="566" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A566" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B566" s="50" t="s">
         <v>598</v>
@@ -23129,7 +23123,7 @@
     </row>
     <row r="567" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A567" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B567" s="50" t="s">
         <v>599</v>
@@ -23137,7 +23131,7 @@
     </row>
     <row r="568" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A568" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B568" s="50" t="s">
         <v>600</v>
@@ -23145,7 +23139,7 @@
     </row>
     <row r="569" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A569" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B569" s="50" t="s">
         <v>601</v>
@@ -23153,7 +23147,7 @@
     </row>
     <row r="570" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A570" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B570" s="50" t="s">
         <v>602</v>
@@ -23161,7 +23155,7 @@
     </row>
     <row r="571" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A571" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B571" s="50" t="s">
         <v>603</v>
@@ -23169,7 +23163,7 @@
     </row>
     <row r="572" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A572" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B572" s="50" t="s">
         <v>604</v>
@@ -23177,7 +23171,7 @@
     </row>
     <row r="573" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A573" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B573" s="50" t="s">
         <v>605</v>
@@ -23185,7 +23179,7 @@
     </row>
     <row r="574" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A574" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B574" s="50" t="s">
         <v>606</v>
@@ -23193,7 +23187,7 @@
     </row>
     <row r="575" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A575" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B575" s="50" t="s">
         <v>607</v>
@@ -23201,7 +23195,7 @@
     </row>
     <row r="576" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A576" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B576" s="50" t="s">
         <v>608</v>
@@ -23209,7 +23203,7 @@
     </row>
     <row r="577" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A577" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B577" s="50" t="s">
         <v>609</v>
@@ -23217,7 +23211,7 @@
     </row>
     <row r="578" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A578" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B578" s="50" t="s">
         <v>610</v>
@@ -23225,7 +23219,7 @@
     </row>
     <row r="579" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A579" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B579" s="50" t="s">
         <v>611</v>
@@ -23233,7 +23227,7 @@
     </row>
     <row r="580" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A580" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B580" s="50" t="s">
         <v>612</v>
@@ -23241,7 +23235,7 @@
     </row>
     <row r="581" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A581" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B581" s="50" t="s">
         <v>613</v>
@@ -23249,7 +23243,7 @@
     </row>
     <row r="582" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A582" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B582" s="50" t="s">
         <v>614</v>
@@ -23257,7 +23251,7 @@
     </row>
     <row r="583" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A583" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B583" s="50" t="s">
         <v>615</v>
@@ -23265,7 +23259,7 @@
     </row>
     <row r="584" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A584" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B584" s="50" t="s">
         <v>616</v>
@@ -23273,7 +23267,7 @@
     </row>
     <row r="585" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A585" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B585" s="50" t="s">
         <v>617</v>
@@ -23281,7 +23275,7 @@
     </row>
     <row r="586" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A586" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B586" s="50" t="s">
         <v>618</v>
@@ -23289,7 +23283,7 @@
     </row>
     <row r="587" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A587" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B587" s="50" t="s">
         <v>619</v>
@@ -23297,7 +23291,7 @@
     </row>
     <row r="588" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A588" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B588" s="50" t="s">
         <v>620</v>
@@ -23305,7 +23299,7 @@
     </row>
     <row r="589" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A589" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B589" s="50" t="s">
         <v>621</v>
@@ -23313,7 +23307,7 @@
     </row>
     <row r="590" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A590" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B590" s="50" t="s">
         <v>622</v>
@@ -23321,7 +23315,7 @@
     </row>
     <row r="591" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A591" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B591" s="50" t="s">
         <v>623</v>
@@ -23329,7 +23323,7 @@
     </row>
     <row r="592" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A592" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B592" s="50" t="s">
         <v>624</v>
@@ -23337,7 +23331,7 @@
     </row>
     <row r="593" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A593" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B593" s="50" t="s">
         <v>625</v>
@@ -23345,7 +23339,7 @@
     </row>
     <row r="594" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A594" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B594" s="50" t="s">
         <v>626</v>
@@ -23353,7 +23347,7 @@
     </row>
     <row r="595" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A595" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B595" s="50" t="s">
         <v>627</v>
@@ -23361,7 +23355,7 @@
     </row>
     <row r="596" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A596" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B596" s="50" t="s">
         <v>628</v>
@@ -23369,7 +23363,7 @@
     </row>
     <row r="597" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A597" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B597" s="50" t="s">
         <v>629</v>
@@ -23377,7 +23371,7 @@
     </row>
     <row r="598" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A598" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B598" s="50" t="s">
         <v>630</v>
@@ -23385,31 +23379,31 @@
     </row>
     <row r="599" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A599" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B599" s="50" t="s">
-        <v>631</v>
+        <v>66</v>
       </c>
     </row>
     <row r="600" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A600" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B600" s="50" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="601" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A601" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B601" s="50" t="s">
-        <v>66</v>
+        <v>632</v>
       </c>
     </row>
     <row r="602" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A602" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B602" s="50" t="s">
         <v>633</v>
@@ -23417,7 +23411,7 @@
     </row>
     <row r="603" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A603" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B603" s="50" t="s">
         <v>634</v>
@@ -23425,7 +23419,7 @@
     </row>
     <row r="604" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A604" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B604" s="50" t="s">
         <v>635</v>
@@ -23433,7 +23427,7 @@
     </row>
     <row r="605" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A605" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B605" s="50" t="s">
         <v>636</v>
@@ -23441,7 +23435,7 @@
     </row>
     <row r="606" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A606" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B606" s="50" t="s">
         <v>637</v>
@@ -23449,7 +23443,7 @@
     </row>
     <row r="607" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A607" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B607" s="50" t="s">
         <v>638</v>
@@ -23457,7 +23451,7 @@
     </row>
     <row r="608" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A608" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B608" s="50" t="s">
         <v>639</v>
@@ -23465,7 +23459,7 @@
     </row>
     <row r="609" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A609" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B609" s="50" t="s">
         <v>640</v>
@@ -23473,7 +23467,7 @@
     </row>
     <row r="610" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A610" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B610" s="50" t="s">
         <v>641</v>
@@ -23481,7 +23475,7 @@
     </row>
     <row r="611" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A611" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B611" s="50" t="s">
         <v>642</v>
@@ -23489,7 +23483,7 @@
     </row>
     <row r="612" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A612" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B612" s="50" t="s">
         <v>643</v>
@@ -23497,7 +23491,7 @@
     </row>
     <row r="613" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A613" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B613" s="50" t="s">
         <v>644</v>
@@ -23505,7 +23499,7 @@
     </row>
     <row r="614" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A614" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B614" s="50" t="s">
         <v>645</v>
@@ -23513,7 +23507,7 @@
     </row>
     <row r="615" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A615" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B615" s="50" t="s">
         <v>646</v>
@@ -23521,7 +23515,7 @@
     </row>
     <row r="616" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A616" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B616" s="50" t="s">
         <v>647</v>
@@ -23529,7 +23523,7 @@
     </row>
     <row r="617" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A617" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B617" s="50" t="s">
         <v>648</v>
@@ -23537,7 +23531,7 @@
     </row>
     <row r="618" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A618" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B618" s="50" t="s">
         <v>649</v>
@@ -23545,7 +23539,7 @@
     </row>
     <row r="619" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A619" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B619" s="50" t="s">
         <v>650</v>
@@ -23553,7 +23547,7 @@
     </row>
     <row r="620" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A620" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B620" s="50" t="s">
         <v>651</v>
@@ -23561,7 +23555,7 @@
     </row>
     <row r="621" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A621" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B621" s="50" t="s">
         <v>652</v>
@@ -23569,7 +23563,7 @@
     </row>
     <row r="622" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A622" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B622" s="50" t="s">
         <v>653</v>
@@ -23577,7 +23571,7 @@
     </row>
     <row r="623" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A623" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B623" s="50" t="s">
         <v>654</v>
@@ -23585,7 +23579,7 @@
     </row>
     <row r="624" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A624" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B624" s="50" t="s">
         <v>655</v>
@@ -23593,7 +23587,7 @@
     </row>
     <row r="625" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A625" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B625" s="50" t="s">
         <v>656</v>
@@ -23601,7 +23595,7 @@
     </row>
     <row r="626" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A626" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B626" s="50" t="s">
         <v>657</v>
@@ -23609,7 +23603,7 @@
     </row>
     <row r="627" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A627" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B627" s="50" t="s">
         <v>658</v>
@@ -23617,7 +23611,7 @@
     </row>
     <row r="628" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A628" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B628" s="50" t="s">
         <v>659</v>
@@ -23625,7 +23619,7 @@
     </row>
     <row r="629" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A629" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B629" s="50" t="s">
         <v>660</v>
@@ -23633,7 +23627,7 @@
     </row>
     <row r="630" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A630" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B630" s="50" t="s">
         <v>661</v>
@@ -23641,7 +23635,7 @@
     </row>
     <row r="631" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A631" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B631" s="50" t="s">
         <v>662</v>
@@ -23649,7 +23643,7 @@
     </row>
     <row r="632" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A632" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B632" s="50" t="s">
         <v>663</v>
@@ -23657,7 +23651,7 @@
     </row>
     <row r="633" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A633" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B633" s="50" t="s">
         <v>664</v>
@@ -23665,7 +23659,7 @@
     </row>
     <row r="634" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A634" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B634" s="50" t="s">
         <v>665</v>
@@ -23673,7 +23667,7 @@
     </row>
     <row r="635" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A635" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B635" s="50" t="s">
         <v>666</v>
@@ -23681,7 +23675,7 @@
     </row>
     <row r="636" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A636" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B636" s="50" t="s">
         <v>667</v>
@@ -23689,7 +23683,7 @@
     </row>
     <row r="637" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A637" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B637" s="50" t="s">
         <v>668</v>
@@ -23697,7 +23691,7 @@
     </row>
     <row r="638" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A638" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B638" s="50" t="s">
         <v>669</v>
@@ -23705,7 +23699,7 @@
     </row>
     <row r="639" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A639" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B639" s="50" t="s">
         <v>670</v>
@@ -23713,7 +23707,7 @@
     </row>
     <row r="640" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A640" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B640" s="50" t="s">
         <v>671</v>
@@ -23721,7 +23715,7 @@
     </row>
     <row r="641" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A641" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B641" s="50" t="s">
         <v>672</v>
@@ -23729,7 +23723,7 @@
     </row>
     <row r="642" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A642" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B642" s="50" t="s">
         <v>673</v>
@@ -23737,7 +23731,7 @@
     </row>
     <row r="643" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A643" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B643" s="50" t="s">
         <v>674</v>
@@ -23745,7 +23739,7 @@
     </row>
     <row r="644" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A644" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B644" s="50" t="s">
         <v>675</v>
@@ -23753,7 +23747,7 @@
     </row>
     <row r="645" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A645" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B645" s="50" t="s">
         <v>676</v>
@@ -23761,7 +23755,7 @@
     </row>
     <row r="646" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A646" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B646" s="50" t="s">
         <v>677</v>
@@ -23769,7 +23763,7 @@
     </row>
     <row r="647" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A647" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B647" s="50" t="s">
         <v>678</v>
@@ -23777,7 +23771,7 @@
     </row>
     <row r="648" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A648" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B648" s="50" t="s">
         <v>679</v>
@@ -23785,7 +23779,7 @@
     </row>
     <row r="649" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A649" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B649" s="50" t="s">
         <v>680</v>
@@ -23793,7 +23787,7 @@
     </row>
     <row r="650" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A650" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B650" s="50" t="s">
         <v>681</v>
@@ -23801,7 +23795,7 @@
     </row>
     <row r="651" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A651" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B651" s="50" t="s">
         <v>682</v>
@@ -23809,7 +23803,7 @@
     </row>
     <row r="652" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A652" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B652" s="50" t="s">
         <v>683</v>
@@ -23817,7 +23811,7 @@
     </row>
     <row r="653" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A653" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B653" s="50" t="s">
         <v>684</v>
@@ -23825,7 +23819,7 @@
     </row>
     <row r="654" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A654" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B654" s="50" t="s">
         <v>685</v>
@@ -23833,7 +23827,7 @@
     </row>
     <row r="655" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A655" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B655" s="50" t="s">
         <v>686</v>
@@ -23841,7 +23835,7 @@
     </row>
     <row r="656" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A656" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B656" s="50" t="s">
         <v>687</v>
@@ -23849,7 +23843,7 @@
     </row>
     <row r="657" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A657" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B657" s="50" t="s">
         <v>688</v>
@@ -23857,7 +23851,7 @@
     </row>
     <row r="658" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A658" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B658" s="50" t="s">
         <v>689</v>
@@ -23865,7 +23859,7 @@
     </row>
     <row r="659" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A659" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B659" s="50" t="s">
         <v>690</v>
@@ -23873,7 +23867,7 @@
     </row>
     <row r="660" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A660" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B660" s="50" t="s">
         <v>691</v>
@@ -23881,7 +23875,7 @@
     </row>
     <row r="661" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A661" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B661" s="50" t="s">
         <v>692</v>
@@ -23889,7 +23883,7 @@
     </row>
     <row r="662" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A662" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B662" s="50" t="s">
         <v>693</v>
@@ -23897,7 +23891,7 @@
     </row>
     <row r="663" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A663" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B663" s="50" t="s">
         <v>694</v>
@@ -23905,7 +23899,7 @@
     </row>
     <row r="664" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A664" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B664" s="50" t="s">
         <v>695</v>
@@ -23913,7 +23907,7 @@
     </row>
     <row r="665" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A665" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B665" s="50" t="s">
         <v>696</v>
@@ -23921,7 +23915,7 @@
     </row>
     <row r="666" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A666" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B666" s="50" t="s">
         <v>697</v>
@@ -23929,7 +23923,7 @@
     </row>
     <row r="667" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A667" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B667" s="50" t="s">
         <v>698</v>
@@ -23937,7 +23931,7 @@
     </row>
     <row r="668" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A668" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B668" s="50" t="s">
         <v>699</v>
@@ -23945,7 +23939,7 @@
     </row>
     <row r="669" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A669" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B669" s="50" t="s">
         <v>700</v>
@@ -23953,7 +23947,7 @@
     </row>
     <row r="670" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A670" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B670" s="50" t="s">
         <v>701</v>
@@ -23961,7 +23955,7 @@
     </row>
     <row r="671" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A671" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B671" s="50" t="s">
         <v>702</v>
@@ -23969,7 +23963,7 @@
     </row>
     <row r="672" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A672" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B672" s="50" t="s">
         <v>703</v>
@@ -23977,26 +23971,26 @@
     </row>
     <row r="673" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A673" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B673" s="50" t="s">
         <v>704</v>
       </c>
     </row>
-    <row r="674" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A674" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="B674" s="50" t="s">
+    <row r="676" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A676" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B676" s="51" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="675" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A675" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="B675" s="50" t="s">
-        <v>706</v>
+    <row r="677" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A677" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B677" s="51" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="678" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -24004,23 +23998,7 @@
         <v>15</v>
       </c>
       <c r="B678" s="51" t="s">
-        <v>707</v>
-      </c>
-    </row>
-    <row r="679" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A679" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B679" s="51" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="680" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A680" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B680" s="51" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
     </row>
   </sheetData>
@@ -24051,17 +24029,17 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.01171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.03125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="53.04"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="52" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="B1" s="53" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24069,7 +24047,7 @@
         <v>4203</v>
       </c>
       <c r="B2" s="55" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24077,7 +24055,7 @@
         <v>4203100001</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24085,7 +24063,7 @@
         <v>4203100009</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24093,7 +24071,7 @@
         <v>6106</v>
       </c>
       <c r="B5" s="55" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24101,7 +24079,7 @@
         <v>6106100000</v>
       </c>
       <c r="B6" s="56" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24109,7 +24087,7 @@
         <v>6106200000</v>
       </c>
       <c r="B7" s="56" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24117,7 +24095,7 @@
         <v>6106901000</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24125,7 +24103,7 @@
         <v>6106903000</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24133,7 +24111,7 @@
         <v>6106905000</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24141,7 +24119,7 @@
         <v>6106909000</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24149,7 +24127,7 @@
         <v>6201</v>
       </c>
       <c r="B12" s="55" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24157,7 +24135,7 @@
         <v>6201200000</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24165,7 +24143,7 @@
         <v>6201300000</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24173,7 +24151,7 @@
         <v>6201400000</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24181,7 +24159,7 @@
         <v>6201900000</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24189,7 +24167,7 @@
         <v>6202</v>
       </c>
       <c r="B17" s="55" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24197,7 +24175,7 @@
         <v>6202200000</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24205,7 +24183,7 @@
         <v>6202300000</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24213,7 +24191,7 @@
         <v>6202400001</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24221,7 +24199,7 @@
         <v>6202400009</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24229,7 +24207,7 @@
         <v>6202900001</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24237,7 +24215,7 @@
         <v>6202900009</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24245,7 +24223,7 @@
         <v>6302</v>
       </c>
       <c r="B24" s="55" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24253,7 +24231,7 @@
         <v>6302100001</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24261,7 +24239,7 @@
         <v>6302100009</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24269,7 +24247,7 @@
         <v>6302210000</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24277,7 +24255,7 @@
         <v>6302221000</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24285,7 +24263,7 @@
         <v>6302229000</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24293,7 +24271,7 @@
         <v>6302310001</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24301,7 +24279,7 @@
         <v>6302310009</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24309,7 +24287,7 @@
         <v>6302321000</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24317,7 +24295,7 @@
         <v>6302329000</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24325,7 +24303,7 @@
         <v>6302392001</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24333,7 +24311,7 @@
         <v>6302392009</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24341,7 +24319,7 @@
         <v>6302399000</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24349,7 +24327,7 @@
         <v>6302400000</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24357,7 +24335,7 @@
         <v>6302510001</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24365,7 +24343,7 @@
         <v>6302510009</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24373,7 +24351,7 @@
         <v>6302531000</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24381,7 +24359,7 @@
         <v>6302539000</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24389,7 +24367,7 @@
         <v>6302591000</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24397,7 +24375,7 @@
         <v>6302599000</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24405,7 +24383,7 @@
         <v>6302600000</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24413,7 +24391,7 @@
         <v>6302910000</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24421,7 +24399,7 @@
         <v>6302931000</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24429,7 +24407,7 @@
         <v>6302939000</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24437,7 +24415,7 @@
         <v>6302991000</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24445,7 +24423,7 @@
         <v>6302999000</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24453,7 +24431,7 @@
         <v>4303</v>
       </c>
       <c r="B50" s="55" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24461,7 +24439,7 @@
         <v>4303109010</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24469,7 +24447,7 @@
         <v>4303109020</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24477,7 +24455,7 @@
         <v>4303109030</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24485,7 +24463,7 @@
         <v>4303109040</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24493,7 +24471,7 @@
         <v>4303109050</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24501,7 +24479,7 @@
         <v>4303109060</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24509,7 +24487,7 @@
         <v>4303109080</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24517,7 +24495,7 @@
         <v>3303</v>
       </c>
       <c r="B58" s="57" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24525,7 +24503,7 @@
         <v>3303001000</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24533,7 +24511,7 @@
         <v>3303009000</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24541,7 +24519,7 @@
         <v>4011</v>
       </c>
       <c r="B61" s="55" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24549,7 +24527,7 @@
         <v>4011100003</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24557,7 +24535,7 @@
         <v>4011100009</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24565,7 +24543,7 @@
         <v>4011201000</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24573,7 +24551,7 @@
         <v>4011209000</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24581,7 +24559,7 @@
         <v>4011400000</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24589,7 +24567,7 @@
         <v>4011700000</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24597,7 +24575,7 @@
         <v>4011800000</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24605,7 +24583,7 @@
         <v>4011900000</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24613,7 +24591,7 @@
         <v>6401</v>
       </c>
       <c r="B70" s="55" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24621,7 +24599,7 @@
         <v>6401100000</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24629,7 +24607,7 @@
         <v>6401921000</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24637,7 +24615,7 @@
         <v>6401929000</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24645,7 +24623,7 @@
         <v>6401990000</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24653,7 +24631,7 @@
         <v>6402</v>
       </c>
       <c r="B75" s="55" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24661,7 +24639,7 @@
         <v>6402121000</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24669,7 +24647,7 @@
         <v>6402129000</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24677,7 +24655,7 @@
         <v>6402190000</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24685,7 +24663,7 @@
         <v>6402200000</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24693,7 +24671,7 @@
         <v>6402911000</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="26.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24701,7 +24679,7 @@
         <v>6402919000</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24709,7 +24687,7 @@
         <v>6402990500</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24717,7 +24695,7 @@
         <v>6402991000</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="64.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24725,7 +24703,7 @@
         <v>6402993100</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24733,7 +24711,7 @@
         <v>6402993900</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24741,7 +24719,7 @@
         <v>6402995000</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24749,7 +24727,7 @@
         <v>6402999100</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24757,7 +24735,7 @@
         <v>6402999300</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24765,7 +24743,7 @@
         <v>6402999600</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24773,7 +24751,7 @@
         <v>6402999800</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24781,7 +24759,7 @@
         <v>6403</v>
       </c>
       <c r="B91" s="55" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24789,7 +24767,7 @@
         <v>6403120000</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24797,7 +24775,7 @@
         <v>6403190000</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24805,7 +24783,7 @@
         <v>6403200000</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24813,7 +24791,7 @@
         <v>6403400000</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="52.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24821,7 +24799,7 @@
         <v>6403510500</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24829,7 +24807,7 @@
         <v>6403511100</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24837,7 +24815,7 @@
         <v>6403511500</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24845,7 +24823,7 @@
         <v>6403511900</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24853,7 +24831,7 @@
         <v>6403519100</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24861,7 +24839,7 @@
         <v>6403519500</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24869,7 +24847,7 @@
         <v>6403519900</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24877,7 +24855,7 @@
         <v>6403590500</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24885,7 +24863,7 @@
         <v>6403591100</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24893,7 +24871,7 @@
         <v>6403593100</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24901,7 +24879,7 @@
         <v>6403593500</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24909,7 +24887,7 @@
         <v>6403593900</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24917,7 +24895,7 @@
         <v>6403595000</v>
       </c>
       <c r="B108" s="8" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24925,7 +24903,7 @@
         <v>6403599100</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24933,7 +24911,7 @@
         <v>6403599500</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24941,7 +24919,7 @@
         <v>6403599900</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24949,7 +24927,7 @@
         <v>6403910500</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24957,7 +24935,7 @@
         <v>6403911100</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24965,7 +24943,7 @@
         <v>6403911300</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24973,7 +24951,7 @@
         <v>6403911600</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24981,7 +24959,7 @@
         <v>6403911800</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24989,7 +24967,7 @@
         <v>6403919100</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24997,7 +24975,7 @@
         <v>6403919300</v>
       </c>
       <c r="B118" s="8" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25005,7 +24983,7 @@
         <v>6403919600</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25013,7 +24991,7 @@
         <v>6403919800</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25021,7 +24999,7 @@
         <v>6403990500</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25029,7 +25007,7 @@
         <v>6403991100</v>
       </c>
       <c r="B122" s="8" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25037,7 +25015,7 @@
         <v>6403993100</v>
       </c>
       <c r="B123" s="8" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25045,7 +25023,7 @@
         <v>6403993300</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25053,7 +25031,7 @@
         <v>6403993600</v>
       </c>
       <c r="B125" s="8" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25061,7 +25039,7 @@
         <v>6403993800</v>
       </c>
       <c r="B126" s="8" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25069,7 +25047,7 @@
         <v>6403995000</v>
       </c>
       <c r="B127" s="8" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25077,7 +25055,7 @@
         <v>6403999100</v>
       </c>
       <c r="B128" s="8" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25085,7 +25063,7 @@
         <v>6403999300</v>
       </c>
       <c r="B129" s="8" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25093,7 +25071,7 @@
         <v>6403999600</v>
       </c>
       <c r="B130" s="8" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25101,7 +25079,7 @@
         <v>6403999800</v>
       </c>
       <c r="B131" s="8" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25109,7 +25087,7 @@
         <v>6404</v>
       </c>
       <c r="B132" s="55" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25117,7 +25095,7 @@
         <v>6404110000</v>
       </c>
       <c r="B133" s="8" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25125,7 +25103,7 @@
         <v>6404191000</v>
       </c>
       <c r="B134" s="8" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25133,7 +25111,7 @@
         <v>6404199000</v>
       </c>
       <c r="B135" s="8" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25141,7 +25119,7 @@
         <v>6404191000</v>
       </c>
       <c r="B136" s="8" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25149,7 +25127,7 @@
         <v>6404209000</v>
       </c>
       <c r="B137" s="8" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25157,7 +25135,7 @@
         <v>6405</v>
       </c>
       <c r="B138" s="55" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25165,7 +25143,7 @@
         <v>6405100001</v>
       </c>
       <c r="B139" s="8" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25173,7 +25151,7 @@
         <v>6405100009</v>
       </c>
       <c r="B140" s="8" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25181,7 +25159,7 @@
         <v>6405201000</v>
       </c>
       <c r="B141" s="8" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25189,7 +25167,7 @@
         <v>6405209100</v>
       </c>
       <c r="B142" s="8" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25197,7 +25175,7 @@
         <v>6405209900</v>
       </c>
       <c r="B143" s="8" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25205,7 +25183,7 @@
         <v>6405901000</v>
       </c>
       <c r="B144" s="8" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25213,7 +25191,7 @@
         <v>6405909000</v>
       </c>
       <c r="B145" s="8" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
     </row>
   </sheetData>

</xml_diff>